<commit_message>
add template and functionality for new terms
</commit_message>
<xml_diff>
--- a/www/templates/files_manifest.xlsx
+++ b/www/templates/files_manifest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vchung/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAC3B9B-B642-DC42-9037-29C61782975C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34752B9-52F0-024D-875E-350C0C887CCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="460" windowWidth="24120" windowHeight="17540" xr2:uid="{699C1E4D-FBE1-2149-B5D3-FBE286AFA841}"/>
+    <workbookView xWindow="4680" yWindow="5920" windowWidth="24120" windowHeight="12080" xr2:uid="{699C1E4D-FBE1-2149-B5D3-FBE286AFA841}"/>
   </bookViews>
   <sheets>
     <sheet name="manifest" sheetId="1" r:id="rId1"/>

</xml_diff>